<commit_message>
branch test in software tools
</commit_message>
<xml_diff>
--- a/data/org_data/org_data_kenil.xlsx
+++ b/data/org_data/org_data_kenil.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Organization</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>Total Change in Drive Duration</t>
+  </si>
+  <si>
+    <t>Average Time Added to Commute</t>
   </si>
   <si>
     <t>Average Change in Drive Duration</t>
@@ -73,11 +76,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,16 +103,34 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF00CC00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -129,7 +151,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,7 +253,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -244,15 +266,15 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0084D1"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -279,7 +301,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -291,16 +313,561 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="2600">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Number of Employees in Each Organization</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Employees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Org A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Org B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Org C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Org D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Org E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Org F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Org G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Org H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Org I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Org J</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Org K</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Org L</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="10352230"/>
+        <c:axId val="50908998"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10352230"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Organization</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="50908998"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50908998"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Employees</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="10352230"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="2600">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Average Time Added to Commute (West Point, PA)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Time Added to Commute</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0084d1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Org A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Org B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Org C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Org D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Org E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Org F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Org G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Org H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Org I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Org J</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Org K</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Org L</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>29.6814814814867</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.3766793409431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.7397260273966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.0891681627763</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.8180365296834</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.850372208439</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.7638676844855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.6715686274559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47.3734848484909</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.2833333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43.11666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="90362951"/>
+        <c:axId val="22982558"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90362951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="22982558"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22982558"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time Added in Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="90362951"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>786960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>55440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>517680</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>141120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="786960" y="4613400"/>
+        <a:ext cx="10081800" cy="2523960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>74160</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>90360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>722520</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>92880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1009440" y="7086600"/>
+        <a:ext cx="10064160" cy="2440800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -337,10 +904,13 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>45</v>
@@ -349,12 +919,15 @@
         <v>427.7666666664</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>9.50592592592</v>
+        <v>29.6814814814867</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>29.6814814814867</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="n">
         <v>526</v>
@@ -363,12 +936,15 @@
         <v>5412.8666666671</v>
       </c>
       <c r="E5" s="8" t="n">
-        <v>10.2906210392911</v>
+        <v>28.3766793409431</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>28.3766793409431</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>146</v>
@@ -377,12 +953,15 @@
         <v>1353.7833333325</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>9.27248858446918</v>
+        <v>35.7397260273966</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>35.7397260273966</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>557</v>
@@ -391,12 +970,15 @@
         <v>3999.0166666654</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>7.17956313584453</v>
+        <v>26.0891681627763</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>26.0891681627763</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>511</v>
@@ -405,12 +987,15 @@
         <v>3309.0833333336</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>6.4757012394004</v>
+        <v>38.8180365296834</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>38.8180365296834</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7" t="n">
         <v>403</v>
@@ -419,12 +1004,15 @@
         <v>4158.2333333321</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>10.3181968569035</v>
+        <v>23.850372208439</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>23.850372208439</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>131</v>
@@ -433,12 +1021,15 @@
         <v>636.9500000005</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>4.86221374046183</v>
+        <v>33.7638676844855</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>33.7638676844855</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="7" t="n">
         <v>102</v>
@@ -447,12 +1038,15 @@
         <v>649.316666667</v>
       </c>
       <c r="E11" s="8" t="n">
-        <v>6.36584967320589</v>
+        <v>35.6715686274559</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>35.6715686274559</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>22</v>
@@ -460,13 +1054,16 @@
       <c r="D12" s="9" t="n">
         <v>-350.5333333333</v>
       </c>
-      <c r="E12" s="9" t="n">
-        <v>-15.9333333333318</v>
+      <c r="E12" s="5" t="n">
+        <v>47.3734848484909</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>47.3734848484909</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="7" t="n">
         <v>2</v>
@@ -474,13 +1071,16 @@
       <c r="D13" s="10" t="n">
         <v>-2.5333333333</v>
       </c>
-      <c r="E13" s="10" t="n">
-        <v>-1.26666666665</v>
+      <c r="E13" s="8" t="n">
+        <v>53.675</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>53.675</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>6</v>
@@ -489,12 +1089,15 @@
         <v>58.8166666666</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>9.80277777776667</v>
+        <v>21.2833333333333</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>21.2833333333333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="7" t="n">
         <v>2</v>
@@ -503,7 +1106,10 @@
         <v>14.7</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>7.35</v>
+        <v>43.11666666665</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>43.11666666665</v>
       </c>
     </row>
   </sheetData>
@@ -517,5 +1123,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>